<commit_message>
save whylogs htmlstring visualization along with release artifacts
</commit_message>
<xml_diff>
--- a/docs/risk/risk_register.xlsx
+++ b/docs/risk/risk_register.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,6 +628,47 @@
         </is>
       </c>
       <c r="I5" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>80d5083a-00d0-4303-8126-8a0b0cc7ecc3</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-05-18T21:50:58.951381</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
         </is>
@@ -644,7 +685,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -776,6 +817,47 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>80d5083a-00d0-4303-8126-8a0b0cc7ecc3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-05-18T21:50:58.951381</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>bias_protected_groups</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
implement PR suggestions and additional dashboard improvements
</commit_message>
<xml_diff>
--- a/docs/risk/risk_register.xlsx
+++ b/docs/risk/risk_register.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Risks" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="HazardDetails" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Risks" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="HazardDetails" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,10 +18,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -35,7 +43,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -43,15 +51,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -126,9 +152,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -166,7 +192,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -200,6 +226,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -234,9 +261,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -414,7 +442,592 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Run_ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Risk_overall</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Risk_auc</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Risk_bias</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Risk_category</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Risk_description</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Mitigation</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Article</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Mitigation_status</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Review_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>37f94793-eb33-4b87-af40-0bcef324eb69</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-05-16T07:32:18.338074</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2025-05-19T17:01:40.796394</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>c5db13af-71a2-42fd-ba82-bfa034d7e847</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-05-16T07:42:34.763101</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2025-05-19T17:01:40.796394</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>14da633e-fc6f-49e3-99d2-91b1d21fd285</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-05-16T07:46:00.762115</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2025-05-19T17:01:40.796394</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4af71110-b951-44aa-978f-8b07fca405bc</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-05-16T11:25:01.396705</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2025-05-19T17:01:40.796394</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>80d5083a-00d0-4303-8126-8a0b0cc7ecc3</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-05-18T21:50:58.951381</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2025-05-19T17:01:40.796394</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>20449c81-ae32-44ba-bc5e-20cfd92652fb</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-05-19T09:52:25.375210</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2025-05-19T17:01:40.796394</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>d34770bf-1bc0-447f-8505-221ed00e08bc</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-05-19T10:30:47.891257</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2025-05-19T17:01:40.796394</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>545ef4d9-b368-411d-ad35-85266d6220bf</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-05-19T12:30:39.647169</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2025-05-19T17:01:40.796394</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>508880ff-6bc7-428b-8cb2-59f027aade02</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-05-19T16:53:17.469827</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2025-05-19T17:01:40.796394</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,16 +1081,31 @@
           <t>Mitigation</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Article</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Mitigation_status</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Review_date</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>37f94793-eb33-4b87-af40-0bcef324eb69</t>
+          <t>ec007ea6-d722-4914-92e0-426f61a87f6c</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-16T07:32:18.338074</t>
+          <t>2025-05-19T18:57:15.734518</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -509,168 +1137,19 @@
           <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>c5db13af-71a2-42fd-ba82-bfa034d7e847</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-05-16T07:42:34.763101</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0.525</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>PENDING</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Unfair bias against protected demographic groups</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>14da633e-fc6f-49e3-99d2-91b1d21fd285</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-05-16T07:46:00.762115</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0.525</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Unfair bias against protected demographic groups</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4af71110-b951-44aa-978f-8b07fca405bc</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2025-05-16T11:25:01.396705</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0.525</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Unfair bias against protected demographic groups</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>80d5083a-00d0-4303-8126-8a0b0cc7ecc3</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2025-05-18T21:50:58.951381</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0.525</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Unfair bias against protected demographic groups</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2025-05-19T18:57:15.734518</t>
         </is>
       </c>
     </row>
@@ -679,13 +1158,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -734,16 +1213,21 @@
           <t>Details</t>
         </is>
       </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Article</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>14da633e-fc6f-49e3-99d2-91b1d21fd285</t>
+          <t>ec007ea6-d722-4914-92e0-426f61a87f6c</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-16T07:46:00.762115</t>
+          <t>2025-05-19T18:57:15.734518</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -775,86 +1259,9 @@
 </t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>4af71110-b951-44aa-978f-8b07fca405bc</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-05-16T11:25:01.396705</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0.525</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>bias_protected_groups</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Unfair bias against protected demographic groups</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>80d5083a-00d0-4303-8126-8a0b0cc7ecc3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-05-18T21:50:58.951381</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0.525</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>bias_protected_groups</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Unfair bias against protected demographic groups</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
-</t>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>article_10</t>
         </is>
       </c>
     </row>

</xml_diff>